<commit_message>
fix check CheckedSpecialItem UT
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CheckedSpecialDataSample.xlsx
+++ b/CloudTest/SampleData/CheckedSpecialDataSample.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\emr-cloud-be(new)\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceCode\SmartKarte_1\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AAF519-E622-41C6-B8F6-0CE7E645D41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="15" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_INF" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
     <sheet name="PT_HOKEN_PATTERN" sheetId="16" r:id="rId15"/>
     <sheet name="PT_ROUSAI_TENKI" sheetId="14" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1437,7 +1436,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
@@ -1788,11 +1787,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A206C908-B73B-4F57-9BEE-2DB1C5F880C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,6 +1800,7 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="28.5703125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
@@ -1811,7 +1811,7 @@
     <col min="16" max="16" width="15.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" customWidth="1"/>
     <col min="22" max="22" width="12.140625" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
     <col min="26" max="26" width="16.42578125" customWidth="1"/>
@@ -2010,7 +2010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AAFF5E-1553-423A-8948-5BABD26D3D84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2118,7 +2118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EA7E5D-5876-4E84-8E29-B9F2D3C3E653}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2341,7 +2341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2892F96D-4BBB-4A2B-89D1-DCE074D5AF81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2495,7 +2495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39969BAD-2255-4590-A481-753CD7492ECB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2653,7 +2653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC06F9-B56A-49DC-8DA6-70D5C7DCEB9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -2701,7 +2701,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E6173B-2B54-4FD6-BDDC-E47DE7F4F556}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -2854,10 +2854,10 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80339B3E-C46C-4F5F-965E-FBFD75439185}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2962,7 +2962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904BF98-9085-4855-9DF7-31BF552F8ACF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3116,7 +3116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C64218F-649F-4F64-9498-4695D5FE04D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5164,7 +5164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A7406A-BC0C-494B-AAF4-B33C0F46F337}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5288,7 +5288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33C15FF-8821-4889-9140-0A2EC07A7D73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5394,7 +5394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B309D67-BB97-4939-A394-3B8E99A0D15B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -5575,7 +5575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14A4ED8-8CA4-4E5D-B593-9F16E6D3AF8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5948,7 +5948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0689A42-EE24-40E3-9D61-7FAA08A3308D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6277,7 +6277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D721056-BF6E-4B9A-B45A-56D46289D5AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>